<commit_message>
Model Changes for Inclination
Added a workaround to Mission Definitions to select between two JSON files based upon inclination.  Updates all Vehicle Optimization Tables accordingly.
</commit_message>
<xml_diff>
--- a/Vehicle Optimization Tables JS&R_small.xlsx
+++ b/Vehicle Optimization Tables JS&R_small.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chelm\Documents\WorkingFolder\ProjectRoot\projects\GMAT\GMAT-Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8CE2B8-CAF5-4344-89B2-F6A0464DEEBC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79FDB04-1F56-47E0-83EF-E9B91F2BD0CF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11835" tabRatio="983" firstSheet="4" activeTab="10" xr2:uid="{B46CED55-D31E-4830-8707-8BA8DF62075B}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11835" tabRatio="983" firstSheet="4" activeTab="4" xr2:uid="{B46CED55-D31E-4830-8707-8BA8DF62075B}"/>
   </bookViews>
   <sheets>
     <sheet name="Revisions" sheetId="48" r:id="rId1"/>
@@ -10168,7 +10168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0D97AB-4AF0-493E-80E8-592CB4A9EE45}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -22293,8 +22293,8 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22503,7 +22503,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>51.2</v>
+        <v>51.6</v>
       </c>
       <c r="C17">
         <v>-0.64</v>

</xml_diff>